<commit_message>
Added code for email bounce chart
</commit_message>
<xml_diff>
--- a/files/excel/CMPG-A2-LD2-11122025.xlsx
+++ b/files/excel/CMPG-A2-LD2-11122025.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1500" yWindow="1500" windowWidth="17280" windowHeight="8880" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -16,7 +16,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -62,6 +62,20 @@
       <family val="2"/>
       <color rgb="FF000000"/>
       <sz val="11"/>
+    </font>
+    <font>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+      <color rgb="FF0072C6"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="10"/>
+      <sz val="11"/>
+      <u val="single"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -129,10 +143,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -149,9 +164,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -526,10 +544,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H96"/>
+  <dimension ref="A1:O96"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="I96" sqref="I96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
@@ -541,6 +559,7 @@
     <col width="40.44140625" customWidth="1" min="6" max="6"/>
     <col width="33.33203125" customWidth="1" min="7" max="7"/>
     <col width="24.6640625" customWidth="1" min="8" max="8"/>
+    <col width="18" customWidth="1" min="9" max="9"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -555,7 +574,7 @@
         </is>
       </c>
     </row>
-    <row r="2">
+    <row r="2" ht="15" customHeight="1">
       <c r="A2" s="1" t="inlineStr">
         <is>
           <t>HTML File Name</t>
@@ -564,6 +583,11 @@
       <c r="B2" t="inlineStr">
         <is>
           <t>CMPG-11122025.html</t>
+        </is>
+      </c>
+      <c r="O2" s="8" t="inlineStr">
+        <is>
+          <t>chaitanya.kumar@axisbank.com</t>
         </is>
       </c>
     </row>
@@ -578,6 +602,11 @@
           <t xml:space="preserve"> Support Your Team’s Growth with Better Learning</t>
         </is>
       </c>
+      <c r="O3" s="9" t="inlineStr">
+        <is>
+          <t>ajeesh.mathew@esafbank.com</t>
+        </is>
+      </c>
     </row>
     <row r="4" ht="15" customHeight="1" thickBot="1">
       <c r="C4" s="2" t="inlineStr">
@@ -608,6 +637,16 @@
       <c r="H4" s="2" t="inlineStr">
         <is>
           <t>Status</t>
+        </is>
+      </c>
+      <c r="I4" s="2" t="inlineStr">
+        <is>
+          <t>Bounce Back Mails</t>
+        </is>
+      </c>
+      <c r="O4" s="9" t="inlineStr">
+        <is>
+          <t>vdongare@rebit.org.in</t>
         </is>
       </c>
     </row>
@@ -630,9 +669,12 @@
           <t>eliza.george@mahindrafinance.com</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>Sent email at slno 1 at time: 11/12/2025,19:10:03</t>
+      <c r="I5" t="b">
+        <v>0</v>
+      </c>
+      <c r="O5" s="9" t="inlineStr">
+        <is>
+          <t>avinashk@cybage.com</t>
         </is>
       </c>
     </row>
@@ -655,9 +697,12 @@
           <t>chetanb@hdfcsales.com</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>Sent email at slno 2 at time: 11/12/2025,19:10:09</t>
+      <c r="I6" t="b">
+        <v>0</v>
+      </c>
+      <c r="O6" s="9" t="inlineStr">
+        <is>
+          <t>shraddha.thakur@tcs.com</t>
         </is>
       </c>
     </row>
@@ -680,9 +725,12 @@
           <t>anu.yermal@kotak.com</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>Sent email at slno 3 at time: 11/12/2025,19:11:49</t>
+      <c r="I7" t="b">
+        <v>0</v>
+      </c>
+      <c r="O7" s="9" t="inlineStr">
+        <is>
+          <t>hemanth.prabhu@hp.com</t>
         </is>
       </c>
     </row>
@@ -705,10 +753,8 @@
           <t>sudeshnar@hdfclife.com</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>Sent email at slno 4 at time: 11/12/2025,19:11:56</t>
-        </is>
+      <c r="I8" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="9" ht="15" customHeight="1" thickBot="1">
@@ -730,10 +776,8 @@
           <t>ameeta.sawant@hdbfs.com</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>Sent email at slno 5 at time: 11/12/2025,19:12:02</t>
-        </is>
+      <c r="I9" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="10" ht="15" customHeight="1" thickBot="1">
@@ -755,10 +799,8 @@
           <t>ajeesh.mathew@esafbank.com</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>Sent email at slno 6 at time: 11/12/2025,19:12:06</t>
-        </is>
+      <c r="I10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="11" ht="15" customHeight="1" thickBot="1">
@@ -780,10 +822,8 @@
           <t>rs.wadhawa@sbi.co.in</t>
         </is>
       </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>Sent email at slno 7 at time: 11/12/2025,19:12:11</t>
-        </is>
+      <c r="I11" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="12" ht="15" customHeight="1" thickBot="1">
@@ -805,10 +845,8 @@
           <t>tuhina.rani@broadridge.com</t>
         </is>
       </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>Sent email at slno 8 at time: 11/12/2025,19:12:16</t>
-        </is>
+      <c r="I12" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="13" ht="15" customHeight="1" thickBot="1">
@@ -830,10 +868,8 @@
           <t>vijaykorath@sib.co.in</t>
         </is>
       </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>Sent email at slno 9 at time: 11/12/2025,19:12:20</t>
-        </is>
+      <c r="I13" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="14" ht="15" customHeight="1" thickBot="1">
@@ -855,10 +891,8 @@
           <t>mahima.singh@avendus.com</t>
         </is>
       </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>Sent email at slno 10 at time: 11/12/2025,19:12:27</t>
-        </is>
+      <c r="I14" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="15" ht="15" customHeight="1" thickBot="1">
@@ -880,10 +914,8 @@
           <t>bhawna.piplani@aavas.in</t>
         </is>
       </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>Sent email at slno 11 at time: 11/12/2025,19:12:31</t>
-        </is>
+      <c r="I15" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="16" ht="15" customHeight="1" thickBot="1">
@@ -905,10 +937,8 @@
           <t>surabhi.sontakke@bajajfinserv.in</t>
         </is>
       </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>Sent email at slno 12 at time: 11/12/2025,19:12:37</t>
-        </is>
+      <c r="I16" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="17" ht="15" customHeight="1" thickBot="1">
@@ -930,10 +960,8 @@
           <t>deepika.ethirajan@sc.com</t>
         </is>
       </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>Sent email at slno 13 at time: 11/12/2025,19:12:40</t>
-        </is>
+      <c r="I17" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="18" ht="15" customHeight="1" thickBot="1">
@@ -955,10 +983,8 @@
           <t>aabied.mansoori@kotak.com</t>
         </is>
       </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>Sent email at slno 14 at time: 11/12/2025,19:12:47</t>
-        </is>
+      <c r="I18" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="19" ht="15" customHeight="1" thickBot="1">
@@ -980,10 +1006,8 @@
           <t>nishant_rathore@mas.co.in</t>
         </is>
       </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>Sent email at slno 15 at time: 11/12/2025,19:12:51</t>
-        </is>
+      <c r="I19" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="20" ht="15" customHeight="1" thickBot="1">
@@ -1005,10 +1029,8 @@
           <t>ram.matlani@tatacapital.com</t>
         </is>
       </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>Sent email at slno 16 at time: 11/12/2025,19:12:56</t>
-        </is>
+      <c r="I20" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="21" ht="15" customHeight="1" thickBot="1">
@@ -1030,10 +1052,8 @@
           <t>raju.k@angelone.in</t>
         </is>
       </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>Sent email at slno 17 at time: 11/12/2025,19:13:00</t>
-        </is>
+      <c r="I21" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="22" ht="15" customHeight="1" thickBot="1">
@@ -1055,10 +1075,8 @@
           <t>chaitanya.kumar@axisbank.com</t>
         </is>
       </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>Sent email at slno 18 at time: 11/12/2025,19:13:05</t>
-        </is>
+      <c r="I22" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="23" ht="15" customHeight="1" thickBot="1">
@@ -1080,10 +1098,8 @@
           <t>shalu.priya@yesbank.in</t>
         </is>
       </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>Sent email at slno 19 at time: 11/12/2025,19:13:09</t>
-        </is>
+      <c r="I23" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="24" ht="15" customHeight="1" thickBot="1">
@@ -1105,10 +1121,8 @@
           <t>prasanths@hdfcsales.com</t>
         </is>
       </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>Sent email at slno 20 at time: 11/12/2025,19:13:14</t>
-        </is>
+      <c r="I24" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="25" ht="15" customHeight="1" thickBot="1">
@@ -1130,10 +1144,8 @@
           <t>rakesh.hazra@bandhanbank.com</t>
         </is>
       </c>
-      <c r="H25" t="inlineStr">
-        <is>
-          <t>Sent email at slno 21 at time: 11/12/2025,19:13:19</t>
-        </is>
+      <c r="I25" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="26" ht="15" customHeight="1" thickBot="1">
@@ -1155,10 +1167,8 @@
           <t>pratik@sbfc.com</t>
         </is>
       </c>
-      <c r="H26" t="inlineStr">
-        <is>
-          <t>Sent email at slno 22 at time: 11/12/2025,19:13:23</t>
-        </is>
+      <c r="I26" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="27" ht="15" customHeight="1" thickBot="1">
@@ -1180,10 +1190,8 @@
           <t>joseph.t@onelearn.global</t>
         </is>
       </c>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t>Sent email at slno 23 at time: 11/12/2025,19:13:28</t>
-        </is>
+      <c r="I27" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="28" ht="15" customHeight="1" thickBot="1">
@@ -1205,10 +1213,8 @@
           <t>nandini.nair@cognizant.com</t>
         </is>
       </c>
-      <c r="H28" t="inlineStr">
-        <is>
-          <t>Sent email at slno 24 at time: 11/12/2025,19:13:31</t>
-        </is>
+      <c r="I28" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="29" ht="15" customHeight="1" thickBot="1">
@@ -1230,10 +1236,8 @@
           <t>bhavisha.kapadia@axisbank.com</t>
         </is>
       </c>
-      <c r="H29" t="inlineStr">
-        <is>
-          <t>Sent email at slno 25 at time: 11/12/2025,19:13:36</t>
-        </is>
+      <c r="I29" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="30" ht="15" customHeight="1" thickBot="1">
@@ -1255,10 +1259,8 @@
           <t>anna.autade@morganstanley.com</t>
         </is>
       </c>
-      <c r="H30" t="inlineStr">
-        <is>
-          <t>Sent email at slno 26 at time: 11/12/2025,19:13:40</t>
-        </is>
+      <c r="I30" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="31" ht="15" customHeight="1" thickBot="1">
@@ -1280,10 +1282,8 @@
           <t>sakshi.dhiman@genpact.com</t>
         </is>
       </c>
-      <c r="H31" t="inlineStr">
-        <is>
-          <t>Sent email at slno 27 at time: 11/12/2025,19:13:44</t>
-        </is>
+      <c r="I31" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="32" ht="15" customHeight="1" thickBot="1">
@@ -1305,10 +1305,8 @@
           <t>mshaw@tracelink.com</t>
         </is>
       </c>
-      <c r="H32" t="inlineStr">
-        <is>
-          <t>Sent email at slno 28 at time: 11/12/2025,19:13:48</t>
-        </is>
+      <c r="I32" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="33" ht="15" customHeight="1" thickBot="1">
@@ -1330,10 +1328,8 @@
           <t>nishad.mehta@larsentoubro.com</t>
         </is>
       </c>
-      <c r="H33" t="inlineStr">
-        <is>
-          <t>Sent email at slno 29 at time: 11/12/2025,19:13:52</t>
-        </is>
+      <c r="I33" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="34" ht="15" customHeight="1" thickBot="1">
@@ -1355,10 +1351,8 @@
           <t>nehaghosh@bluestarindia.com</t>
         </is>
       </c>
-      <c r="H34" t="inlineStr">
-        <is>
-          <t>Sent email at slno 30 at time: 11/12/2025,19:13:56</t>
-        </is>
+      <c r="I34" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="35" ht="15" customHeight="1" thickBot="1">
@@ -1380,10 +1374,8 @@
           <t>madhuri.venkatesh@sodexo.com</t>
         </is>
       </c>
-      <c r="H35" t="inlineStr">
-        <is>
-          <t>Sent email at slno 31 at time: 11/12/2025,19:14:00</t>
-        </is>
+      <c r="I35" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="36" ht="15" customHeight="1" thickBot="1">
@@ -1405,10 +1397,8 @@
           <t>swati.pandey@bajajallianz.co.in</t>
         </is>
       </c>
-      <c r="H36" t="inlineStr">
-        <is>
-          <t>Sent email at slno 32 at time: 11/12/2025,19:14:04</t>
-        </is>
+      <c r="I36" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="37" ht="15" customHeight="1" thickBot="1">
@@ -1430,10 +1420,8 @@
           <t>shrija@bmes.com</t>
         </is>
       </c>
-      <c r="H37" t="inlineStr">
-        <is>
-          <t>Sent email at slno 33 at time: 11/12/2025,19:14:08</t>
-        </is>
+      <c r="I37" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="38" ht="15" customHeight="1" thickBot="1">
@@ -1455,10 +1443,8 @@
           <t>kalyan.balantrapu@accenture.com</t>
         </is>
       </c>
-      <c r="H38" t="inlineStr">
-        <is>
-          <t>Sent email at slno 34 at time: 11/12/2025,19:14:13</t>
-        </is>
+      <c r="I38" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="39" ht="15" customHeight="1" thickBot="1">
@@ -1480,10 +1466,8 @@
           <t>sanya.kataria1@aexp.com</t>
         </is>
       </c>
-      <c r="H39" t="inlineStr">
-        <is>
-          <t>Sent email at slno 35 at time: 11/12/2025,19:14:16</t>
-        </is>
+      <c r="I39" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="40" ht="15" customHeight="1" thickBot="1">
@@ -1505,10 +1489,8 @@
           <t>suchana.misra@marriott.com</t>
         </is>
       </c>
-      <c r="H40" t="inlineStr">
-        <is>
-          <t>Sent email at slno 36 at time: 11/12/2025,19:14:21</t>
-        </is>
+      <c r="I40" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="41" ht="15" customHeight="1" thickBot="1">
@@ -1530,10 +1512,8 @@
           <t>ankit.mahendra@paytm.com</t>
         </is>
       </c>
-      <c r="H41" t="inlineStr">
-        <is>
-          <t>Sent email at slno 37 at time: 11/12/2025,19:14:25</t>
-        </is>
+      <c r="I41" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="42" ht="15" customHeight="1" thickBot="1">
@@ -1555,10 +1535,8 @@
           <t>sjena@deloitte.com</t>
         </is>
       </c>
-      <c r="H42" t="inlineStr">
-        <is>
-          <t>Sent email at slno 38 at time: 11/12/2025,19:14:29</t>
-        </is>
+      <c r="I42" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="43" ht="15" customHeight="1" thickBot="1">
@@ -1580,10 +1558,8 @@
           <t>rao.nikhil@bcg.com</t>
         </is>
       </c>
-      <c r="H43" t="inlineStr">
-        <is>
-          <t>Sent email at slno 39 at time: 11/12/2025,19:14:33</t>
-        </is>
+      <c r="I43" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="44" ht="15" customHeight="1" thickBot="1">
@@ -1605,10 +1581,8 @@
           <t>devika.mitra@leixir.com</t>
         </is>
       </c>
-      <c r="H44" t="inlineStr">
-        <is>
-          <t>Sent email at slno 40 at time: 11/12/2025,19:14:38</t>
-        </is>
+      <c r="I44" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="45" ht="15" customHeight="1" thickBot="1">
@@ -1630,10 +1604,8 @@
           <t>ankita.pahwa@tajhotels.com</t>
         </is>
       </c>
-      <c r="H45" t="inlineStr">
-        <is>
-          <t>Sent email at slno 41 at time: 11/12/2025,19:14:42</t>
-        </is>
+      <c r="I45" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="46" ht="15" customHeight="1" thickBot="1">
@@ -1655,10 +1627,8 @@
           <t>prateek.gupta@adityabirla.com</t>
         </is>
       </c>
-      <c r="H46" t="inlineStr">
-        <is>
-          <t>Sent email at slno 42 at time: 11/12/2025,19:14:46</t>
-        </is>
+      <c r="I46" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="47" ht="15" customHeight="1" thickBot="1">
@@ -1680,10 +1650,8 @@
           <t>sreenath@sapphireglobal.biz</t>
         </is>
       </c>
-      <c r="H47" t="inlineStr">
-        <is>
-          <t>Sent email at slno 43 at time: 11/12/2025,19:14:50</t>
-        </is>
+      <c r="I47" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="48" ht="15" customHeight="1" thickBot="1">
@@ -1705,10 +1673,8 @@
           <t>mehak.arora@grazitti.com</t>
         </is>
       </c>
-      <c r="H48" t="inlineStr">
-        <is>
-          <t>Sent email at slno 44 at time: 11/12/2025,19:14:54</t>
-        </is>
+      <c r="I48" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="49" ht="15" customHeight="1" thickBot="1">
@@ -1730,10 +1696,8 @@
           <t>ambika.srivastava@nbcbearings.in</t>
         </is>
       </c>
-      <c r="H49" t="inlineStr">
-        <is>
-          <t>Sent email at slno 45 at time: 11/12/2025,19:14:58</t>
-        </is>
+      <c r="I49" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="50" ht="15" customHeight="1" thickBot="1">
@@ -1755,10 +1719,8 @@
           <t>manmeet.narang@avaada.com</t>
         </is>
       </c>
-      <c r="H50" t="inlineStr">
-        <is>
-          <t>Sent email at slno 46 at time: 11/12/2025,19:15:03</t>
-        </is>
+      <c r="I50" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="51" ht="15" customHeight="1" thickBot="1">
@@ -1780,10 +1742,8 @@
           <t>deepak.arora@birlasoft.com</t>
         </is>
       </c>
-      <c r="H51" t="inlineStr">
-        <is>
-          <t>Sent email at slno 47 at time: 11/12/2025,19:15:06</t>
-        </is>
+      <c r="I51" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="52" ht="15" customHeight="1" thickBot="1">
@@ -1805,10 +1765,8 @@
           <t>diya.sajan@eclinicalworks.com</t>
         </is>
       </c>
-      <c r="H52" t="inlineStr">
-        <is>
-          <t>Sent email at slno 48 at time: 11/12/2025,19:15:11</t>
-        </is>
+      <c r="I52" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="53" ht="15" customHeight="1" thickBot="1">
@@ -1830,10 +1788,8 @@
           <t>rohit.shenoy@dxc.com</t>
         </is>
       </c>
-      <c r="H53" t="inlineStr">
-        <is>
-          <t>Sent email at slno 49 at time: 11/12/2025,19:15:14</t>
-        </is>
+      <c r="I53" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="54" ht="15" customHeight="1" thickBot="1">
@@ -1855,10 +1811,8 @@
           <t>jaya.ethiraj@aspiresys.com</t>
         </is>
       </c>
-      <c r="H54" t="inlineStr">
-        <is>
-          <t>Sent email at slno 50 at time: 11/12/2025,19:15:18</t>
-        </is>
+      <c r="I54" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="55" ht="15" customHeight="1" thickBot="1">
@@ -1880,10 +1834,8 @@
           <t>faisal.tanveer@kbr.com</t>
         </is>
       </c>
-      <c r="H55" t="inlineStr">
-        <is>
-          <t>Sent email at slno 51 at time: 11/12/2025,19:15:22</t>
-        </is>
+      <c r="I55" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="56" ht="15" customHeight="1" thickBot="1">
@@ -1905,10 +1857,8 @@
           <t>swathip@coreflexsolutions.com</t>
         </is>
       </c>
-      <c r="H56" t="inlineStr">
-        <is>
-          <t>Sent email at slno 52 at time: 11/12/2025,19:15:26</t>
-        </is>
+      <c r="I56" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="57" ht="15" customHeight="1" thickBot="1">
@@ -1930,10 +1880,8 @@
           <t>smaniyar@capgemini.com</t>
         </is>
       </c>
-      <c r="H57" t="inlineStr">
-        <is>
-          <t>Sent email at slno 53 at time: 11/12/2025,19:15:30</t>
-        </is>
+      <c r="I57" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="58" ht="15" customHeight="1" thickBot="1">
@@ -1955,10 +1903,8 @@
           <t>suraj.bhatia@lancesoft.com</t>
         </is>
       </c>
-      <c r="H58" t="inlineStr">
-        <is>
-          <t>Sent email at slno 54 at time: 11/12/2025,19:15:34</t>
-        </is>
+      <c r="I58" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="59" ht="15" customHeight="1" thickBot="1">
@@ -1980,10 +1926,8 @@
           <t>amita_sawant@persistent.co.in</t>
         </is>
       </c>
-      <c r="H59" t="inlineStr">
-        <is>
-          <t>Sent email at slno 55 at time: 11/12/2025,19:15:41</t>
-        </is>
+      <c r="I59" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="60" ht="15" customHeight="1" thickBot="1">
@@ -2005,10 +1949,8 @@
           <t>arunbabu@qburst.com</t>
         </is>
       </c>
-      <c r="H60" t="inlineStr">
-        <is>
-          <t>Sent email at slno 56 at time: 11/12/2025,19:15:47</t>
-        </is>
+      <c r="I60" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="61" ht="15" customHeight="1" thickBot="1">
@@ -2030,10 +1972,8 @@
           <t>vdongare@rebit.org.in</t>
         </is>
       </c>
-      <c r="H61" t="inlineStr">
-        <is>
-          <t>Sent email at slno 57 at time: 11/12/2025,19:15:51</t>
-        </is>
+      <c r="I61" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="62" ht="15" customHeight="1" thickBot="1">
@@ -2055,10 +1995,8 @@
           <t>sonam.shrimal@i2econsulting.com</t>
         </is>
       </c>
-      <c r="H62" t="inlineStr">
-        <is>
-          <t>Sent email at slno 58 at time: 11/12/2025,19:15:56</t>
-        </is>
+      <c r="I62" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="63" ht="15" customHeight="1" thickBot="1">
@@ -2080,10 +2018,8 @@
           <t>william.meshy@innovasolutions.com</t>
         </is>
       </c>
-      <c r="H63" t="inlineStr">
-        <is>
-          <t>Sent email at slno 59 at time: 11/12/2025,19:16:00</t>
-        </is>
+      <c r="I63" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="64" ht="15" customHeight="1" thickBot="1">
@@ -2105,10 +2041,8 @@
           <t>roshni.arora@wipro.com</t>
         </is>
       </c>
-      <c r="H64" t="inlineStr">
-        <is>
-          <t>Sent email at slno 60 at time: 11/12/2025,19:16:05</t>
-        </is>
+      <c r="I64" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="65" ht="15" customHeight="1" thickBot="1">
@@ -2130,10 +2064,8 @@
           <t>aman.singh@collabera.com</t>
         </is>
       </c>
-      <c r="H65" t="inlineStr">
-        <is>
-          <t>Sent email at slno 61 at time: 11/12/2025,19:16:09</t>
-        </is>
+      <c r="I65" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="66" ht="15" customHeight="1" thickBot="1">
@@ -2155,10 +2087,8 @@
           <t>vikas.khandelwal@fiserv.com</t>
         </is>
       </c>
-      <c r="H66" t="inlineStr">
-        <is>
-          <t>Sent email at slno 62 at time: 11/12/2025,19:16:13</t>
-        </is>
+      <c r="I66" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="67" ht="15" customHeight="1" thickBot="1">
@@ -2180,10 +2110,8 @@
           <t>devis@hexaware.com</t>
         </is>
       </c>
-      <c r="H67" t="inlineStr">
-        <is>
-          <t>Sent email at slno 63 at time: 11/12/2025,19:16:18</t>
-        </is>
+      <c r="I67" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="68" ht="15" customHeight="1" thickBot="1">
@@ -2205,10 +2133,8 @@
           <t>gayathiri.ramkumar@tatatechnologies.com</t>
         </is>
       </c>
-      <c r="H68" t="inlineStr">
-        <is>
-          <t>Sent email at slno 64 at time: 11/12/2025,19:16:22</t>
-        </is>
+      <c r="I68" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="69" ht="15" customHeight="1" thickBot="1">
@@ -2230,10 +2156,8 @@
           <t>yogesh.tawde@esds.co.in</t>
         </is>
       </c>
-      <c r="H69" t="inlineStr">
-        <is>
-          <t>Sent email at slno 65 at time: 11/12/2025,19:16:26</t>
-        </is>
+      <c r="I69" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="70" ht="15" customHeight="1" thickBot="1">
@@ -2255,10 +2179,8 @@
           <t>nihal.velani@accelya.com</t>
         </is>
       </c>
-      <c r="H70" t="inlineStr">
-        <is>
-          <t>Sent email at slno 66 at time: 11/12/2025,19:16:30</t>
-        </is>
+      <c r="I70" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="71" ht="15" customHeight="1" thickBot="1">
@@ -2280,10 +2202,8 @@
           <t>rajshree_ahirrao@persistent.co.in</t>
         </is>
       </c>
-      <c r="H71" t="inlineStr">
-        <is>
-          <t>Sent email at slno 67 at time: 11/12/2025,19:16:35</t>
-        </is>
+      <c r="I71" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="72" ht="15" customHeight="1" thickBot="1">
@@ -2305,10 +2225,8 @@
           <t>chanchal.sharma@mivada.com</t>
         </is>
       </c>
-      <c r="H72" t="inlineStr">
-        <is>
-          <t>Sent email at slno 68 at time: 11/12/2025,19:16:40</t>
-        </is>
+      <c r="I72" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="73" ht="15" customHeight="1" thickBot="1">
@@ -2330,10 +2248,8 @@
           <t>boney.antony@brillio.com</t>
         </is>
       </c>
-      <c r="H73" t="inlineStr">
-        <is>
-          <t>Sent email at slno 69 at time: 11/12/2025,19:16:44</t>
-        </is>
+      <c r="I73" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="74" ht="15" customHeight="1" thickBot="1">
@@ -2355,10 +2271,8 @@
           <t>sonam.chauhan@irissoftware.com</t>
         </is>
       </c>
-      <c r="H74" t="inlineStr">
-        <is>
-          <t>Sent email at slno 70 at time: 11/12/2025,19:16:48</t>
-        </is>
+      <c r="I74" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="75" ht="15" customHeight="1" thickBot="1">
@@ -2380,10 +2294,8 @@
           <t>karan.gupta@coforge.com</t>
         </is>
       </c>
-      <c r="H75" t="inlineStr">
-        <is>
-          <t>Sent email at slno 71 at time: 11/12/2025,19:16:52</t>
-        </is>
+      <c r="I75" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="76" ht="15" customHeight="1" thickBot="1">
@@ -2405,10 +2317,8 @@
           <t>pushpanath.dasika@blackbox.com</t>
         </is>
       </c>
-      <c r="H76" t="inlineStr">
-        <is>
-          <t>Sent email at slno 72 at time: 11/12/2025,19:16:58</t>
-        </is>
+      <c r="I76" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="77" ht="15" customHeight="1" thickBot="1">
@@ -2430,10 +2340,8 @@
           <t>preeti.bahl@coforge.com</t>
         </is>
       </c>
-      <c r="H77" t="inlineStr">
-        <is>
-          <t>Sent email at slno 73 at time: 11/12/2025,19:17:04</t>
-        </is>
+      <c r="I77" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="78" ht="15" customHeight="1" thickBot="1">
@@ -2455,10 +2363,8 @@
           <t>hemanth.prabhu@hp.com</t>
         </is>
       </c>
-      <c r="H78" t="inlineStr">
-        <is>
-          <t>Sent email at slno 74 at time: 11/12/2025,19:17:09</t>
-        </is>
+      <c r="I78" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="79" ht="15" customHeight="1" thickBot="1">
@@ -2480,10 +2386,8 @@
           <t>varsha@accenture.com</t>
         </is>
       </c>
-      <c r="H79" t="inlineStr">
-        <is>
-          <t>Sent email at slno 75 at time: 11/12/2025,19:17:15</t>
-        </is>
+      <c r="I79" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="80" ht="15" customHeight="1" thickBot="1">
@@ -2505,10 +2409,8 @@
           <t>thomas.koshy@ust-global.com</t>
         </is>
       </c>
-      <c r="H80" t="inlineStr">
-        <is>
-          <t>Sent email at slno 76 at time: 11/12/2025,19:17:19</t>
-        </is>
+      <c r="I80" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="81" ht="15" customHeight="1" thickBot="1">
@@ -2530,10 +2432,8 @@
           <t>kamalpreet.kaur@eclerx.com</t>
         </is>
       </c>
-      <c r="H81" t="inlineStr">
-        <is>
-          <t>Sent email at slno 77 at time: 11/12/2025,19:17:23</t>
-        </is>
+      <c r="I81" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="82" ht="15" customHeight="1" thickBot="1">
@@ -2555,10 +2455,8 @@
           <t>mohan.rao@rapyder.com</t>
         </is>
       </c>
-      <c r="H82" t="inlineStr">
-        <is>
-          <t>Sent email at slno 78 at time: 11/12/2025,19:17:28</t>
-        </is>
+      <c r="I82" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="83" ht="15" customHeight="1" thickBot="1">
@@ -2580,10 +2478,8 @@
           <t>manu.sondhi@concentrix.com</t>
         </is>
       </c>
-      <c r="H83" t="inlineStr">
-        <is>
-          <t>Sent email at slno 79 at time: 11/12/2025,19:17:33</t>
-        </is>
+      <c r="I83" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="84" ht="15" customHeight="1" thickBot="1">
@@ -2605,10 +2501,8 @@
           <t>sanchaita.banerjee@mercer.com</t>
         </is>
       </c>
-      <c r="H84" t="inlineStr">
-        <is>
-          <t>Sent email at slno 80 at time: 11/12/2025,19:17:37</t>
-        </is>
+      <c r="I84" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="85" ht="15" customHeight="1" thickBot="1">
@@ -2630,10 +2524,8 @@
           <t>jason.sequeira@quantiphi.com</t>
         </is>
       </c>
-      <c r="H85" t="inlineStr">
-        <is>
-          <t>Sent email at slno 81 at time: 11/12/2025,19:17:41</t>
-        </is>
+      <c r="I85" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="86" ht="15" customHeight="1" thickBot="1">
@@ -2655,10 +2547,8 @@
           <t>merina@leegality.com</t>
         </is>
       </c>
-      <c r="H86" t="inlineStr">
-        <is>
-          <t>Sent email at slno 82 at time: 11/12/2025,19:17:45</t>
-        </is>
+      <c r="I86" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="87" ht="15" customHeight="1" thickBot="1">
@@ -2680,10 +2570,8 @@
           <t>akhila.ali@senecaglobal.com</t>
         </is>
       </c>
-      <c r="H87" t="inlineStr">
-        <is>
-          <t>Sent email at slno 83 at time: 11/12/2025,19:17:50</t>
-        </is>
+      <c r="I87" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="88" ht="15" customHeight="1" thickBot="1">
@@ -2705,10 +2593,8 @@
           <t>srikanth.mosalikante@evolutyz.com</t>
         </is>
       </c>
-      <c r="H88" t="inlineStr">
-        <is>
-          <t>Sent email at slno 84 at time: 11/12/2025,19:17:53</t>
-        </is>
+      <c r="I88" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="89" ht="15" customHeight="1" thickBot="1">
@@ -2730,10 +2616,8 @@
           <t>kanak.ohdar@koantek.com</t>
         </is>
       </c>
-      <c r="H89" t="inlineStr">
-        <is>
-          <t>Sent email at slno 85 at time: 11/12/2025,19:17:58</t>
-        </is>
+      <c r="I89" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="90" ht="15" customHeight="1" thickBot="1">
@@ -2755,10 +2639,8 @@
           <t>neha.tewari@medtronic.com</t>
         </is>
       </c>
-      <c r="H90" t="inlineStr">
-        <is>
-          <t>Sent email at slno 86 at time: 11/12/2025,19:18:02</t>
-        </is>
+      <c r="I90" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="91" ht="15" customHeight="1" thickBot="1">
@@ -2780,10 +2662,8 @@
           <t>kapil.pursnani@ascendion.com</t>
         </is>
       </c>
-      <c r="H91" t="inlineStr">
-        <is>
-          <t>Sent email at slno 87 at time: 11/12/2025,19:18:07</t>
-        </is>
+      <c r="I91" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="92" ht="15" customHeight="1" thickBot="1">
@@ -2805,10 +2685,8 @@
           <t>pranesh.dixit@qualitestgroup.com</t>
         </is>
       </c>
-      <c r="H92" t="inlineStr">
-        <is>
-          <t>Sent email at slno 88 at time: 11/12/2025,19:18:14</t>
-        </is>
+      <c r="I92" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="93" ht="15" customHeight="1" thickBot="1">
@@ -2830,10 +2708,8 @@
           <t>avinashk@cybage.com</t>
         </is>
       </c>
-      <c r="H93" t="inlineStr">
-        <is>
-          <t>Sent email at slno 89 at time: 11/12/2025,19:18:22</t>
-        </is>
+      <c r="I93" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="94" ht="15" customHeight="1" thickBot="1">
@@ -2855,10 +2731,8 @@
           <t>deepti.singh@here.com</t>
         </is>
       </c>
-      <c r="H94" t="inlineStr">
-        <is>
-          <t>Sent email at slno 90 at time: 11/12/2025,19:18:29</t>
-        </is>
+      <c r="I94" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="95" ht="15" customHeight="1" thickBot="1">
@@ -2880,10 +2754,8 @@
           <t>nawaneet.gautam@sapiens.com</t>
         </is>
       </c>
-      <c r="H95" t="inlineStr">
-        <is>
-          <t>Sent email at slno 91 at time: 11/12/2025,19:18:32</t>
-        </is>
+      <c r="I95" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="96" ht="15" customHeight="1" thickBot="1">
@@ -2905,13 +2777,18 @@
           <t>shraddha.thakur@tcs.com</t>
         </is>
       </c>
-      <c r="H96" t="inlineStr">
-        <is>
-          <t>Sent email at slno 92 at time: 11/12/2025,19:18:37</t>
-        </is>
+      <c r="I96" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O3" display="mailto:ajeesh.mathew@esafbank.com" r:id="rId1"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O4" display="mailto:vdongare@rebit.org.in" r:id="rId2"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O5" r:id="rId3"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O6" display="mailto:shraddha.thakur@tcs.com" r:id="rId4"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O7" display="mailto:hemanth.prabhu@hp.com" r:id="rId5"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>